<commit_message>
Checking and slight changes -Cooper
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djraymond\PycharmProjects\cs151-sky-donovan_cooper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nmare\PycharmProjects\cs151-sky-donovan_cooper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C871038-993E-43A7-9E99-0BD930237E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073A9F4E-70F8-4441-BF3B-1E768674BCE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="2352" yWindow="3672" windowWidth="17280" windowHeight="10008" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -536,16 +536,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714008D9-644A-2B47-9D77-29A0AE074340}">
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -560,7 +560,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -581,7 +581,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -602,7 +602,7 @@
       <c r="J3" s="4"/>
       <c r="K3" s="3"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -623,7 +623,7 @@
       <c r="J4" s="4"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -636,7 +636,7 @@
       <c r="J5" s="4"/>
       <c r="K5" s="3"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -649,7 +649,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
@@ -670,7 +670,7 @@
       <c r="J7" s="9"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -703,7 +703,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -727,7 +727,7 @@
         <v>3.0639443699324591</v>
       </c>
       <c r="H9" s="2">
-        <f>C9 C9*G9</f>
+        <f>C9*G9</f>
         <v>61.278887398649182</v>
       </c>
       <c r="I9" s="2">
@@ -740,7 +740,7 @@
       </c>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
@@ -777,7 +777,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
@@ -814,7 +814,7 @@
       </c>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>

</xml_diff>